<commit_message>
Organized root a little. Made Asana csv into xlsx for ones that I won't pull later. removed things that docs don't follow from documentation standards. added docs used for project tracking to logs. added testing log to logs. updated my entry in project_contributors.xlsx
</commit_message>
<xml_diff>
--- a/php/root/logs/hours/project_contributors.xlsx
+++ b/php/root/logs/hours/project_contributors.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sarah Johnston\Dropbox\cp317\group\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\CP317_MLS_Project\php\root\logs\hours\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="164">
   <si>
     <t>Email</t>
   </si>
@@ -514,6 +514,9 @@
   </si>
   <si>
     <t>1. Wrapper documentation (requirements, analysis, design). 2. QA and updating other documentation to reflect changes in later steps, as well as consistency in HTML formatting</t>
+  </si>
+  <si>
+    <t>All docs, all php and python (mainly php). In depth testing of php and python</t>
   </si>
 </sst>
 </file>
@@ -598,7 +601,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -615,6 +618,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1089,7 +1093,7 @@
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1133,749 +1137,751 @@
     </row>
     <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>122</v>
+        <v>33</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>123</v>
+        <v>21</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>124</v>
+        <v>82</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>96</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="G2" s="1">
-        <v>103.7</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>156</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="H2" s="7"/>
     </row>
     <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>32</v>
+        <v>122</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>123</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>124</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E3" s="1"/>
+        <v>151</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>96</v>
+      </c>
       <c r="F3" s="1" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="G3" s="1">
-        <v>81.78</v>
+        <v>103.7</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G4" s="1">
+        <v>81.78</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B5" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="G4" s="1">
-        <v>61.5</v>
-      </c>
-      <c r="H4" s="7"/>
-    </row>
-    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1" t="s">
-        <v>107</v>
-      </c>
       <c r="G5" s="1">
-        <v>50.44</v>
-      </c>
-      <c r="H5" s="7"/>
+        <v>200</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G6" s="1">
-        <v>47.73</v>
+        <v>50.44</v>
       </c>
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>77</v>
+        <v>42</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>78</v>
+        <v>43</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>100</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G7" s="1">
+        <v>47.73</v>
+      </c>
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G8" s="1">
         <v>44</v>
       </c>
-      <c r="H7" s="7"/>
-    </row>
-    <row r="8" spans="1:8" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+      <c r="H8" s="7"/>
+    </row>
+    <row r="9" spans="1:8" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="2" t="s">
+      <c r="E9" s="1"/>
+      <c r="F9" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G9" s="1">
         <v>40.65</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H9" s="7" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="G9" s="1">
-        <v>38.869999999999997</v>
-      </c>
-      <c r="H9" s="7"/>
     </row>
     <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>53</v>
+        <v>89</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>54</v>
+        <v>90</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>147</v>
+        <v>91</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="E10" s="1"/>
-      <c r="F10" s="2" t="s">
-        <v>129</v>
+      <c r="F10" s="1" t="s">
+        <v>117</v>
       </c>
       <c r="G10" s="1">
-        <v>37.78</v>
+        <v>38.869999999999997</v>
       </c>
       <c r="H10" s="7"/>
     </row>
     <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>99</v>
+        <v>55</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="2" t="s">
+        <v>129</v>
       </c>
       <c r="G11" s="1">
-        <v>34.46</v>
+        <v>37.78</v>
       </c>
       <c r="H11" s="7"/>
     </row>
     <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>16</v>
+        <v>63</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>2</v>
+        <v>64</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E12" s="1"/>
+        <v>100</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>96</v>
+      </c>
       <c r="F12" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="G12" s="1">
-        <v>32.119999999999997</v>
+        <v>34.46</v>
       </c>
       <c r="H12" s="7"/>
     </row>
     <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>86</v>
+        <v>28</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>87</v>
+        <v>16</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>88</v>
+        <v>2</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>105</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="G13" s="1">
-        <v>32</v>
+        <v>32.119999999999997</v>
       </c>
       <c r="H13" s="7"/>
     </row>
     <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>47</v>
+        <v>86</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>48</v>
+        <v>87</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>49</v>
+        <v>88</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>105</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="G14" s="1">
-        <v>31.31</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>159</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="H14" s="7"/>
     </row>
     <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>145</v>
+        <v>47</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>146</v>
+        <v>48</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>143</v>
+        <v>49</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="E15" s="1"/>
-      <c r="F15" s="2" t="s">
-        <v>144</v>
+      <c r="F15" s="1" t="s">
+        <v>112</v>
       </c>
       <c r="G15" s="1">
-        <v>29</v>
-      </c>
-      <c r="H15" s="7"/>
+        <v>31.31</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>101</v>
       </c>
       <c r="E16" s="1"/>
-      <c r="F16" s="1" t="s">
-        <v>142</v>
+      <c r="F16" s="2" t="s">
+        <v>144</v>
       </c>
       <c r="G16" s="1">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="H16" s="7"/>
     </row>
     <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>27</v>
+        <v>140</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>15</v>
+        <v>141</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1</v>
+        <v>139</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
       <c r="G17" s="1">
-        <v>25.49</v>
+        <v>26</v>
       </c>
       <c r="H17" s="7"/>
     </row>
     <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>65</v>
+        <v>27</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>67</v>
+        <v>1</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1" t="s">
-        <v>155</v>
+        <v>111</v>
       </c>
       <c r="G18" s="1">
-        <v>23.37</v>
+        <v>25.49</v>
       </c>
       <c r="H18" s="7"/>
     </row>
     <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1" t="s">
-        <v>121</v>
+        <v>155</v>
       </c>
       <c r="G19" s="1">
-        <v>19.5</v>
+        <v>23.37</v>
       </c>
       <c r="H19" s="7"/>
     </row>
     <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>23</v>
+        <v>74</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>8</v>
+        <v>75</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="G20" s="1">
-        <v>17</v>
+        <v>19.5</v>
       </c>
       <c r="H20" s="7"/>
     </row>
     <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>92</v>
+        <v>35</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>93</v>
+        <v>23</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>94</v>
+        <v>8</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>105</v>
+        <v>147</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1" t="s">
-        <v>152</v>
+        <v>118</v>
       </c>
       <c r="G21" s="1">
-        <v>16.45</v>
-      </c>
-      <c r="H21" s="6" t="s">
-        <v>160</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="H21" s="7"/>
     </row>
     <row r="22" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>38</v>
+        <v>92</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>39</v>
+        <v>93</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>12</v>
+        <v>94</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1" t="s">
-        <v>115</v>
+        <v>152</v>
       </c>
       <c r="G22" s="1">
-        <v>16.43</v>
+        <v>16.45</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="G23" s="1">
-        <v>14.95</v>
-      </c>
-      <c r="H23" s="7"/>
+        <v>16.43</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="24" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>101</v>
+        <v>52</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="E24" s="1"/>
-      <c r="F24" s="2" t="s">
-        <v>130</v>
+      <c r="F24" s="1" t="s">
+        <v>119</v>
       </c>
       <c r="G24" s="1">
-        <v>12.28</v>
+        <v>14.95</v>
       </c>
       <c r="H24" s="7"/>
     </row>
     <row r="25" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>101</v>
       </c>
       <c r="E25" s="1"/>
-      <c r="F25" s="1" t="s">
-        <v>113</v>
+      <c r="F25" s="2" t="s">
+        <v>130</v>
       </c>
       <c r="G25" s="1">
-        <v>10.3</v>
+        <v>12.28</v>
       </c>
       <c r="H25" s="7"/>
     </row>
     <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>68</v>
+        <v>22</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>69</v>
+        <v>7</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>101</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="G26" s="1">
-        <v>7.58</v>
-      </c>
-      <c r="H26" s="6" t="s">
-        <v>162</v>
-      </c>
+        <v>10.3</v>
+      </c>
+      <c r="H26" s="7"/>
     </row>
     <row r="27" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="G27" s="1">
-        <v>7</v>
-      </c>
-      <c r="H27" s="7"/>
+        <v>7.58</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="28" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>137</v>
+      <c r="A28" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>147</v>
+        <v>100</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1" t="s">
-        <v>138</v>
+        <v>103</v>
       </c>
       <c r="G28" s="1">
-        <v>5.65</v>
+        <v>7</v>
       </c>
       <c r="H28" s="7"/>
     </row>
     <row r="29" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>9</v>
+      <c r="A29" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>137</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>131</v>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1" t="s">
+        <v>138</v>
       </c>
       <c r="G29" s="1">
-        <v>3</v>
+        <v>5.65</v>
       </c>
       <c r="H29" s="7"/>
     </row>
     <row r="30" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>56</v>
+        <v>24</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1" t="s">
-        <v>98</v>
+      <c r="E30" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="G30" s="1">
-        <v>2.5299999999999998</v>
+        <v>3</v>
       </c>
       <c r="H30" s="7"/>
     </row>
     <row r="31" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>101</v>
+        <v>58</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>147</v>
       </c>
       <c r="E31" s="1"/>
-      <c r="F31" s="2" t="s">
-        <v>133</v>
+      <c r="F31" s="1" t="s">
+        <v>98</v>
       </c>
       <c r="G31" s="1">
-        <v>2.4500000000000002</v>
+        <v>2.5299999999999998</v>
       </c>
       <c r="H31" s="7"/>
     </row>
     <row r="32" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>40</v>
+        <v>79</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>26</v>
+        <v>80</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D32" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>101</v>
       </c>
       <c r="E32" s="1"/>
-      <c r="F32" s="1" t="s">
-        <v>116</v>
+      <c r="F32" s="2" t="s">
+        <v>133</v>
       </c>
       <c r="G32" s="1">
-        <v>1</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="H32" s="7"/>
     </row>
     <row r="33" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>72</v>
+        <v>11</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>150</v>
+        <v>101</v>
       </c>
       <c r="E33" s="1"/>
-      <c r="F33" s="2" t="s">
-        <v>128</v>
+      <c r="F33" s="1" t="s">
+        <v>116</v>
       </c>
       <c r="G33" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H33" s="7"/>
     </row>
     <row r="34" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>33</v>
+        <v>70</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>150</v>
       </c>
       <c r="E34" s="1"/>
-      <c r="F34" s="1" t="s">
-        <v>109</v>
+      <c r="F34" s="2" t="s">
+        <v>128</v>
       </c>
       <c r="G34" s="1">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="H34" s="7"/>
     </row>
@@ -1925,20 +1931,20 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C17" r:id="rId1" xr:uid="{B884118B-5C1F-46B2-B164-E4127B433FA3}"/>
-    <hyperlink ref="C12" r:id="rId2" xr:uid="{91755641-9C0B-46BD-8AB8-B5078C4DD6DD}"/>
+    <hyperlink ref="C18" r:id="rId1" xr:uid="{B884118B-5C1F-46B2-B164-E4127B433FA3}"/>
+    <hyperlink ref="C13" r:id="rId2" xr:uid="{91755641-9C0B-46BD-8AB8-B5078C4DD6DD}"/>
     <hyperlink ref="C36" r:id="rId3" xr:uid="{16D75473-1274-48D1-953D-A4F2322407C1}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{80A7D289-6340-49AB-8CBF-1816DDEC6528}"/>
-    <hyperlink ref="C8" r:id="rId5" xr:uid="{615EBE90-6E29-482D-8B03-8EC4D94B7699}"/>
-    <hyperlink ref="C3" r:id="rId6" xr:uid="{7EB3C320-9937-475B-A164-3BEA7A77CFDA}"/>
-    <hyperlink ref="C34" r:id="rId7" display="hodg4890@mylaurier,ca" xr:uid="{F8CAB213-975A-4175-823C-0A1656C6FFFB}"/>
-    <hyperlink ref="C25" r:id="rId8" xr:uid="{B3D8D251-EF4D-4DDA-864C-EDD89272C56A}"/>
-    <hyperlink ref="C20" r:id="rId9" xr:uid="{6A907BE4-C86E-4F4D-B414-07DADE89318F}"/>
-    <hyperlink ref="C29" r:id="rId10" xr:uid="{41F6FAB0-EA83-4C79-9BDC-FF47B81646AE}"/>
-    <hyperlink ref="C24" r:id="rId11" xr:uid="{2E6BD660-294A-4D0D-B9AA-122C74C1D65A}"/>
-    <hyperlink ref="C32" r:id="rId12" xr:uid="{EAB680F6-F547-4A7C-8467-1E25DC54A84F}"/>
-    <hyperlink ref="C22" r:id="rId13" xr:uid="{0312253E-4111-4EEA-8BAB-9954C118A53E}"/>
-    <hyperlink ref="B4" r:id="rId14" display="https://www.facebook.com/profile.php?id=100009426511342&amp;fref=gc&amp;dti=983789738312185" xr:uid="{8E811273-D9C3-42FE-9D3D-75DE2BBC308D}"/>
+    <hyperlink ref="C6" r:id="rId4" xr:uid="{80A7D289-6340-49AB-8CBF-1816DDEC6528}"/>
+    <hyperlink ref="C9" r:id="rId5" xr:uid="{615EBE90-6E29-482D-8B03-8EC4D94B7699}"/>
+    <hyperlink ref="C4" r:id="rId6" xr:uid="{7EB3C320-9937-475B-A164-3BEA7A77CFDA}"/>
+    <hyperlink ref="C2" r:id="rId7" display="hodg4890@mylaurier,ca" xr:uid="{F8CAB213-975A-4175-823C-0A1656C6FFFB}"/>
+    <hyperlink ref="C26" r:id="rId8" xr:uid="{B3D8D251-EF4D-4DDA-864C-EDD89272C56A}"/>
+    <hyperlink ref="C21" r:id="rId9" xr:uid="{6A907BE4-C86E-4F4D-B414-07DADE89318F}"/>
+    <hyperlink ref="C30" r:id="rId10" xr:uid="{41F6FAB0-EA83-4C79-9BDC-FF47B81646AE}"/>
+    <hyperlink ref="C25" r:id="rId11" xr:uid="{2E6BD660-294A-4D0D-B9AA-122C74C1D65A}"/>
+    <hyperlink ref="C33" r:id="rId12" xr:uid="{EAB680F6-F547-4A7C-8467-1E25DC54A84F}"/>
+    <hyperlink ref="C23" r:id="rId13" xr:uid="{0312253E-4111-4EEA-8BAB-9954C118A53E}"/>
+    <hyperlink ref="B5" r:id="rId14" display="https://www.facebook.com/profile.php?id=100009426511342&amp;fref=gc&amp;dti=983789738312185" xr:uid="{8E811273-D9C3-42FE-9D3D-75DE2BBC308D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId15"/>

</xml_diff>